<commit_message>
multi-customer booking and change flight function
</commit_message>
<xml_diff>
--- a/function.xlsx
+++ b/function.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="21560" windowHeight="20180" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="0" windowWidth="21560" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -101,115 +101,115 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>showEmptySeat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>flightdetail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>showTicket/seat/serviceInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>showServiceInventory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add／change／delete service inventory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>showAgencysCutomerList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create／change／delete  route</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>editNoFlyStatus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pessagersReoprt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cashiersReport</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DailyBookingActivity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monthlyBookingActivity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ticketReservation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>serviceReservation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>changeSeat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>changeServiceReservation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>switchSeat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>changeFlight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>customerReport</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>agentReport</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enable／disableAccount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>searchSchedule</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>showAgencyInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>showCustomerInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>editCustomerInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>editAgencyInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add/deleteCustomerFromList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>searchServiceForSchedule</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>showEmptySeat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>flightdetail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>showTicket/seat/serviceInfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>showServiceInventory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>add／change／delete service inventory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>showAgencysCutomerList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>edit/add/deleteCustomerFromList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>create／change／delete  route</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>editNoFlyStatus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pessagersReoprt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cashiersReport</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DailyBookingActivity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>monthlyBookingActivity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ticketReservation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>serviceReservation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>changeSeat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>changeServiceReservation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>switchSeat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>changeFlight</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>customerReport</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>agentReport</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>enable／disableAccount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>searchSchedule</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>showAgencyInfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>showCustomerInfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>editCustomerInfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>editAgencyInfo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -332,8 +332,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -374,7 +378,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="19">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
@@ -383,6 +387,8 @@
     <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -390,6 +396,8 @@
     <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -720,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -775,7 +783,7 @@
     <row r="3" spans="1:9">
       <c r="A3" s="7"/>
       <c r="B3" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -788,7 +796,7 @@
     <row r="4" spans="1:9">
       <c r="A4" s="7"/>
       <c r="B4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -801,7 +809,7 @@
     <row r="5" spans="1:9">
       <c r="A5" s="7"/>
       <c r="B5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -814,7 +822,7 @@
     <row r="6" spans="1:9">
       <c r="A6" s="7"/>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="2"/>
@@ -827,7 +835,7 @@
     <row r="7" spans="1:9">
       <c r="A7" s="7"/>
       <c r="B7" s="5" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="9"/>
@@ -840,7 +848,7 @@
     <row r="8" spans="1:9">
       <c r="A8" s="7"/>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
@@ -866,7 +874,7 @@
     <row r="10" spans="1:9">
       <c r="A10" s="7"/>
       <c r="B10" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="9"/>
@@ -879,7 +887,7 @@
     <row r="11" spans="1:9">
       <c r="A11" s="7"/>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="2"/>
@@ -892,7 +900,7 @@
     <row r="12" spans="1:9">
       <c r="A12" s="7"/>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="2"/>
@@ -905,7 +913,7 @@
     <row r="13" spans="1:9">
       <c r="A13" s="7"/>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -918,7 +926,7 @@
     <row r="14" spans="1:9">
       <c r="A14" s="7"/>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="2"/>
@@ -951,7 +959,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -963,7 +971,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1005,7 +1013,7 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="2"/>
@@ -1018,7 +1026,7 @@
     <row r="23" spans="1:9">
       <c r="A23" s="7"/>
       <c r="B23" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="9"/>
@@ -1057,7 +1065,7 @@
     <row r="26" spans="1:9">
       <c r="A26" s="7"/>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1070,7 +1078,7 @@
     <row r="27" spans="1:9">
       <c r="A27" s="7"/>
       <c r="B27" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1083,7 +1091,7 @@
     <row r="28" spans="1:9">
       <c r="A28" s="7"/>
       <c r="B28" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1096,7 +1104,7 @@
     <row r="29" spans="1:9">
       <c r="A29" s="7"/>
       <c r="B29" s="5" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1135,7 +1143,7 @@
     <row r="32" spans="1:9">
       <c r="A32" s="7"/>
       <c r="B32" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -1174,7 +1182,7 @@
     <row r="35" spans="1:9">
       <c r="A35" s="7"/>
       <c r="B35" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1187,7 +1195,7 @@
     <row r="36" spans="1:9">
       <c r="A36" s="7"/>
       <c r="B36" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1233,7 +1241,7 @@
         <v>17</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="2"/>
@@ -1246,7 +1254,7 @@
     <row r="41" spans="1:9">
       <c r="A41" s="16"/>
       <c r="B41" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -1259,7 +1267,7 @@
     <row r="42" spans="1:9">
       <c r="A42" s="16"/>
       <c r="B42" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -1272,7 +1280,7 @@
     <row r="43" spans="1:9">
       <c r="A43" s="16"/>
       <c r="B43" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -1285,7 +1293,7 @@
     <row r="44" spans="1:9">
       <c r="A44" s="16"/>
       <c r="B44" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -1298,7 +1306,7 @@
     <row r="45" spans="1:9">
       <c r="A45" s="16"/>
       <c r="B45" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>

</xml_diff>